<commit_message>
Ready To go to V1
</commit_message>
<xml_diff>
--- a/Connected Office Dataset.xlsx
+++ b/Connected Office Dataset.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Programming_And_Stuff\Programming\Git\CMPG-323-Project-5-34551875\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67FB0B57-78AD-4869-A103-E13638B286C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85546A95-D307-4F2E-BC23-04F38335A5E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19320" yWindow="1875" windowWidth="19440" windowHeight="15150" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Zone" sheetId="1" r:id="rId1"/>
@@ -140,190 +140,190 @@
     <t>Is Active</t>
   </si>
   <si>
+    <t>D01</t>
+  </si>
+  <si>
+    <t>Front-door Camera</t>
+  </si>
+  <si>
+    <t>Camera</t>
+  </si>
+  <si>
+    <t>Active</t>
+  </si>
+  <si>
+    <t>D02</t>
+  </si>
+  <si>
+    <t>Boiler Temp</t>
+  </si>
+  <si>
+    <t>Temperature Sensor</t>
+  </si>
+  <si>
+    <t>Inactive</t>
+  </si>
+  <si>
+    <t>D03</t>
+  </si>
+  <si>
+    <t>Speed Testing</t>
+  </si>
+  <si>
+    <t>Speed Sensor</t>
+  </si>
+  <si>
+    <t>D04</t>
+  </si>
+  <si>
+    <t>Entry Access</t>
+  </si>
+  <si>
+    <t>Access Control</t>
+  </si>
+  <si>
+    <t>D05</t>
+  </si>
+  <si>
+    <t>Exit Access</t>
+  </si>
+  <si>
+    <t>D06</t>
+  </si>
+  <si>
+    <t>Light Activation</t>
+  </si>
+  <si>
+    <t>Motion Sensor</t>
+  </si>
+  <si>
+    <t>D07</t>
+  </si>
+  <si>
+    <t>D08</t>
+  </si>
+  <si>
+    <t>Aircon Activation</t>
+  </si>
+  <si>
+    <t>D09</t>
+  </si>
+  <si>
+    <t>Assembly Temp</t>
+  </si>
+  <si>
+    <t>CategoryName</t>
+  </si>
+  <si>
+    <t>CategoryDescription</t>
+  </si>
+  <si>
+    <t>C01</t>
+  </si>
+  <si>
+    <t>Sensing</t>
+  </si>
+  <si>
+    <t>This is one of the four key concepts of IoT. A number used to encrypt (or encode) information so that no one can read it. It deals with how machines can sense their environment in many ways</t>
+  </si>
+  <si>
+    <t>C02</t>
+  </si>
+  <si>
+    <t>Computing</t>
+  </si>
+  <si>
+    <t>This is another of the four key enabling IoT concepts. It includes the Cloudand Machine Learning Machine learning (or ML) is a process by which machines can be trained to perform tasks that required humans before. It's based on analysis of lots of data, and it might affect how some IoT devices work. Artificial Intelligence. Here you will find posts that discuss any of these topics. A generic phrase referring to large numbers of computers located somewhere far away and accessed over the internet. For the IoT, computing may be local, done in the same system or building, or in the cloud, with data shipped up to the cloud and then the result shipped back down</t>
+  </si>
+  <si>
+    <t>C03</t>
+  </si>
+  <si>
+    <t>Communicating</t>
+  </si>
+  <si>
+    <t>This is yet another of the four key IoT concepts. The IoT doesn’t happen without lots of communication, and here you’ll find posts that deal with that communication.</t>
+  </si>
+  <si>
+    <t>C04</t>
+  </si>
+  <si>
+    <t>Actuating</t>
+  </si>
+  <si>
+    <t>This is the final IoT concept; it deals with how computers can control other devices. This category includes all posts related to actuation.</t>
+  </si>
+  <si>
+    <t>C05</t>
+  </si>
+  <si>
+    <t>Security</t>
+  </si>
+  <si>
+    <t>Because of the damage that hackers can do – and have already done, this is an enormously important topic for the IoT. Any posts dealing with security can be found in this category.</t>
+  </si>
+  <si>
+    <t>C06</t>
+  </si>
+  <si>
+    <t>Energy</t>
+  </si>
+  <si>
+    <t>Many IoT devices are battery-powered. So it’s important for designers to consider how much energy they consume as they function</t>
+  </si>
+  <si>
+    <t>C07</t>
+  </si>
+  <si>
+    <t>Privacy</t>
+  </si>
+  <si>
+    <t>Keeping data private is also critical for the IoT. Privacy is often lumped in with security, but it’s a distinct topic, and so it has its own category.</t>
+  </si>
+  <si>
+    <t>Sub Category Name</t>
+  </si>
+  <si>
+    <t>Sub Category Description</t>
+  </si>
+  <si>
+    <t>SC01</t>
+  </si>
+  <si>
+    <t>Visual monitoring tool</t>
+  </si>
+  <si>
+    <t>SC02</t>
+  </si>
+  <si>
+    <t>Measuring air temp</t>
+  </si>
+  <si>
+    <t>SC03</t>
+  </si>
+  <si>
+    <t>Monitoring for motion to trigger action</t>
+  </si>
+  <si>
+    <t>SC04</t>
+  </si>
+  <si>
+    <t>Managing access for people entering and exiting the zone</t>
+  </si>
+  <si>
+    <t>SC05</t>
+  </si>
+  <si>
+    <t>Measuring speed of moving object</t>
+  </si>
+  <si>
+    <t>D10</t>
+  </si>
+  <si>
+    <t>Back-door Camera</t>
+  </si>
+  <si>
     <t>Date Installe</t>
-  </si>
-  <si>
-    <t>D01</t>
-  </si>
-  <si>
-    <t>Front-door Camera</t>
-  </si>
-  <si>
-    <t>Camera</t>
-  </si>
-  <si>
-    <t>Active</t>
-  </si>
-  <si>
-    <t>D02</t>
-  </si>
-  <si>
-    <t>Boiler Temp</t>
-  </si>
-  <si>
-    <t>Temperature Sensor</t>
-  </si>
-  <si>
-    <t>Inactive</t>
-  </si>
-  <si>
-    <t>D03</t>
-  </si>
-  <si>
-    <t>Speed Testing</t>
-  </si>
-  <si>
-    <t>Speed Sensor</t>
-  </si>
-  <si>
-    <t>D04</t>
-  </si>
-  <si>
-    <t>Entry Access</t>
-  </si>
-  <si>
-    <t>Access Control</t>
-  </si>
-  <si>
-    <t>D05</t>
-  </si>
-  <si>
-    <t>Exit Access</t>
-  </si>
-  <si>
-    <t>D06</t>
-  </si>
-  <si>
-    <t>Light Activation</t>
-  </si>
-  <si>
-    <t>Motion Sensor</t>
-  </si>
-  <si>
-    <t>D07</t>
-  </si>
-  <si>
-    <t>D08</t>
-  </si>
-  <si>
-    <t>Aircon Activation</t>
-  </si>
-  <si>
-    <t>D09</t>
-  </si>
-  <si>
-    <t>Assembly Temp</t>
-  </si>
-  <si>
-    <t>CategoryName</t>
-  </si>
-  <si>
-    <t>CategoryDescription</t>
-  </si>
-  <si>
-    <t>C01</t>
-  </si>
-  <si>
-    <t>Sensing</t>
-  </si>
-  <si>
-    <t>This is one of the four key concepts of IoT. A number used to encrypt (or encode) information so that no one can read it. It deals with how machines can sense their environment in many ways</t>
-  </si>
-  <si>
-    <t>C02</t>
-  </si>
-  <si>
-    <t>Computing</t>
-  </si>
-  <si>
-    <t>This is another of the four key enabling IoT concepts. It includes the Cloudand Machine Learning Machine learning (or ML) is a process by which machines can be trained to perform tasks that required humans before. It's based on analysis of lots of data, and it might affect how some IoT devices work. Artificial Intelligence. Here you will find posts that discuss any of these topics. A generic phrase referring to large numbers of computers located somewhere far away and accessed over the internet. For the IoT, computing may be local, done in the same system or building, or in the cloud, with data shipped up to the cloud and then the result shipped back down</t>
-  </si>
-  <si>
-    <t>C03</t>
-  </si>
-  <si>
-    <t>Communicating</t>
-  </si>
-  <si>
-    <t>This is yet another of the four key IoT concepts. The IoT doesn’t happen without lots of communication, and here you’ll find posts that deal with that communication.</t>
-  </si>
-  <si>
-    <t>C04</t>
-  </si>
-  <si>
-    <t>Actuating</t>
-  </si>
-  <si>
-    <t>This is the final IoT concept; it deals with how computers can control other devices. This category includes all posts related to actuation.</t>
-  </si>
-  <si>
-    <t>C05</t>
-  </si>
-  <si>
-    <t>Security</t>
-  </si>
-  <si>
-    <t>Because of the damage that hackers can do – and have already done, this is an enormously important topic for the IoT. Any posts dealing with security can be found in this category.</t>
-  </si>
-  <si>
-    <t>C06</t>
-  </si>
-  <si>
-    <t>Energy</t>
-  </si>
-  <si>
-    <t>Many IoT devices are battery-powered. So it’s important for designers to consider how much energy they consume as they function</t>
-  </si>
-  <si>
-    <t>C07</t>
-  </si>
-  <si>
-    <t>Privacy</t>
-  </si>
-  <si>
-    <t>Keeping data private is also critical for the IoT. Privacy is often lumped in with security, but it’s a distinct topic, and so it has its own category.</t>
-  </si>
-  <si>
-    <t>Sub Category Name</t>
-  </si>
-  <si>
-    <t>Sub Category Description</t>
-  </si>
-  <si>
-    <t>SC01</t>
-  </si>
-  <si>
-    <t>Visual monitoring tool</t>
-  </si>
-  <si>
-    <t>SC02</t>
-  </si>
-  <si>
-    <t>Measuring air temp</t>
-  </si>
-  <si>
-    <t>SC03</t>
-  </si>
-  <si>
-    <t>Monitoring for motion to trigger action</t>
-  </si>
-  <si>
-    <t>SC04</t>
-  </si>
-  <si>
-    <t>Managing access for people entering and exiting the zone</t>
-  </si>
-  <si>
-    <t>SC05</t>
-  </si>
-  <si>
-    <t>Measuring speed of moving object</t>
-  </si>
-  <si>
-    <t>D10</t>
-  </si>
-  <si>
-    <t>Back-door Camera</t>
   </si>
 </sst>
 </file>
@@ -374,7 +374,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -469,11 +469,44 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
@@ -487,7 +520,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -805,7 +843,7 @@
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:C10"/>
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -935,18 +973,18 @@
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -969,24 +1007,24 @@
         <v>34</v>
       </c>
       <c r="G1" s="9" t="s">
-        <v>35</v>
+        <v>96</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B2" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="C2" s="4" t="s">
         <v>37</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>38</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>4</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F2" s="11" t="b">
         <v>1</v>
@@ -997,19 +1035,19 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B3" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="C3" s="4" t="s">
         <v>41</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>42</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>7</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F3" s="11" t="b">
         <v>1</v>
@@ -1020,19 +1058,19 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B4" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="C4" s="4" t="s">
         <v>45</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>46</v>
       </c>
       <c r="D4" s="4" t="s">
         <v>10</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F4" s="11" t="b">
         <v>1</v>
@@ -1043,19 +1081,19 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B5" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="C5" s="4" t="s">
         <v>48</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>49</v>
       </c>
       <c r="D5" s="4" t="s">
         <v>13</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F5" s="11" t="b">
         <v>1</v>
@@ -1066,19 +1104,19 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B6" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="B6" s="4" t="s">
-        <v>51</v>
-      </c>
       <c r="C6" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D6" s="4" t="s">
         <v>13</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F6" s="11" t="b">
         <v>0</v>
@@ -1089,19 +1127,19 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B7" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="C7" s="4" t="s">
         <v>53</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>54</v>
       </c>
       <c r="D7" s="4" t="s">
         <v>19</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F7" s="11" t="b">
         <v>0</v>
@@ -1112,19 +1150,19 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B8" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C8" s="4" t="s">
         <v>37</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>38</v>
       </c>
       <c r="D8" s="4" t="s">
         <v>22</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F8" s="11" t="b">
         <v>1</v>
@@ -1135,19 +1173,19 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="B9" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="B9" s="4" t="s">
-        <v>57</v>
-      </c>
       <c r="C9" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D9" s="4" t="s">
         <v>25</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F9" s="11" t="b">
         <v>0</v>
@@ -1157,48 +1195,48 @@
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
+      <c r="A10" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="B10" s="14" t="s">
         <v>58</v>
       </c>
-      <c r="B10" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="C10" s="4" t="s">
+      <c r="C10" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="D10" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="E10" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="D10" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="E10" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="F10" s="11" t="b">
+      <c r="F10" s="15" t="b">
         <v>0</v>
       </c>
-      <c r="G10" s="12">
+      <c r="G10" s="16">
         <v>44584</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="A11" s="17" t="s">
+        <v>94</v>
+      </c>
+      <c r="B11" s="17" t="s">
         <v>95</v>
       </c>
-      <c r="B11" t="s">
-        <v>96</v>
-      </c>
-      <c r="C11" t="s">
+      <c r="C11" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="D11" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="E11" s="17" t="s">
         <v>38</v>
       </c>
-      <c r="D11" t="s">
-        <v>4</v>
-      </c>
-      <c r="E11" t="s">
-        <v>39</v>
-      </c>
-      <c r="F11" t="b">
+      <c r="F11" s="17" t="b">
         <v>1</v>
       </c>
-      <c r="G11" s="13">
+      <c r="G11" s="18">
         <v>44686</v>
       </c>
     </row>
@@ -1225,87 +1263,87 @@
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="C1" s="5" t="s">
         <v>60</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="B2" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="C2" s="8" t="s">
         <v>63</v>
-      </c>
-      <c r="C2" s="8" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="B3" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="C3" s="7" t="s">
         <v>66</v>
-      </c>
-      <c r="C3" s="7" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="B4" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="C4" s="7" t="s">
         <v>69</v>
-      </c>
-      <c r="C4" s="7" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="B5" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="C5" s="7" t="s">
         <v>72</v>
-      </c>
-      <c r="C5" s="7" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="B6" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="C6" s="7" t="s">
         <v>75</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="B7" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="B7" s="7" t="s">
+      <c r="C7" s="7" t="s">
         <v>78</v>
-      </c>
-      <c r="C7" s="7" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="B8" s="7" t="s">
         <v>80</v>
       </c>
-      <c r="B8" s="7" t="s">
+      <c r="C8" s="7" t="s">
         <v>81</v>
-      </c>
-      <c r="C8" s="7" t="s">
-        <v>82</v>
       </c>
     </row>
   </sheetData>
@@ -1318,7 +1356,7 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B2" sqref="B2:B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1337,80 +1375,80 @@
         <v>31</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>83</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="D2" s="4" t="s">
         <v>85</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D3" s="4" t="s">
         <v>87</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="D4" s="4" t="s">
         <v>89</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="D5" s="4" t="s">
         <v>91</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="D6" s="4" t="s">
         <v>93</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>94</v>
       </c>
     </row>
   </sheetData>
@@ -1419,15 +1457,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="7a090801-4708-43a5-9598-e4e2166c002c">
@@ -1443,6 +1472,15 @@
     </SharedWithUsers>
   </documentManagement>
 </p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1669,20 +1707,20 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0A227DC9-4D6F-4F55-89DE-623758C7FB72}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8B45281D-5D5A-4087-8014-4B4FA16E83A5}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="7a090801-4708-43a5-9598-e4e2166c002c"/>
     <ds:schemaRef ds:uri="4f4a8c57-659f-4264-b765-bd165a88863b"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0A227DC9-4D6F-4F55-89DE-623758C7FB72}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>